<commit_message>
modified first xlsx file
</commit_message>
<xml_diff>
--- a/someData.xlsx
+++ b/someData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,8 +11,19 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Kin Id</t>
+  </si>
+  <si>
+    <t>61652_FS</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +353,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
creating milestone on little-feature
</commit_message>
<xml_diff>
--- a/someData.xlsx
+++ b/someData.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Kin Id</t>
-  </si>
-  <si>
-    <t>61652_FS</t>
+    <t>working on little feature</t>
   </si>
 </sst>
 </file>
@@ -353,22 +350,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kin id will be commited
</commit_message>
<xml_diff>
--- a/someData.xlsx
+++ b/someData.xlsx
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Kin Id</t>
   </si>
   <si>
     <t>61652_FS</t>
+  </si>
+  <si>
+    <t>This is in staging area</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -371,6 +374,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>